<commit_message>
my name is sheela
</commit_message>
<xml_diff>
--- a/FirstProject/Global Data Repositories/17c9853c-52dd-411b-94f3-ab93f482a8e4.xlsx
+++ b/FirstProject/Global Data Repositories/17c9853c-52dd-411b-94f3-ab93f482a8e4.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>go to hell</t>
   </si>
@@ -21,6 +21,21 @@
   </si>
   <si>
     <t>HELLO</t>
+  </si>
+  <si>
+    <t>hi</t>
+  </si>
+  <si>
+    <t>my</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is </t>
+  </si>
+  <si>
+    <t>sheela</t>
   </si>
 </sst>
 </file>
@@ -85,8 +100,24 @@
       <c r="D1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" ht="16" customHeight="1"/>
+    <row r="2" ht="16" customHeight="1">
+      <c r="A2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
     <row r="3" ht="16" customHeight="1"/>
     <row r="4" ht="16" customHeight="1"/>
     <row r="5" ht="16" customHeight="1"/>

</xml_diff>